<commit_message>
Adecuacuin de alugnos UML
</commit_message>
<xml_diff>
--- a/Documentacion/Plantilla Historias Usuario - Oficina de Proyectos de Informatica.xlsx
+++ b/Documentacion/Plantilla Historias Usuario - Oficina de Proyectos de Informatica.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIO\Documents\Proyectos\E-vote\E-vote-Backend\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\E-vote\E-vote-Backend\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACAA4A5-4664-47C4-B562-1F40CDDC15F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="317">
   <si>
     <t>Desarrollo ágil: Historias de usuario y criterios de aceptación</t>
   </si>
@@ -1767,12 +1760,15 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Como un candidato</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1812,12 +1808,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2089,20 +2079,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2113,6 +2109,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2120,26 +2121,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2169,7 +2159,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2481,11 +2471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2602,18 +2592,18 @@
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="52" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2725,10 +2715,10 @@
     </row>
     <row r="7" spans="1:26" ht="57" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="17">
         <v>2</v>
       </c>
@@ -2763,10 +2753,10 @@
     </row>
     <row r="8" spans="1:26" ht="131.25" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="17">
         <v>3</v>
       </c>
@@ -2829,16 +2819,16 @@
     </row>
     <row r="10" spans="1:26" ht="45">
       <c r="A10" s="1"/>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="49" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="5">
@@ -2875,10 +2865,10 @@
     </row>
     <row r="11" spans="1:26" ht="52.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="5">
         <v>2</v>
       </c>
@@ -2913,10 +2903,10 @@
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="10">
         <v>3</v>
       </c>
@@ -2951,10 +2941,10 @@
     </row>
     <row r="13" spans="1:26" ht="49.9" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="10">
         <v>4</v>
       </c>
@@ -3017,16 +3007,16 @@
     </row>
     <row r="15" spans="1:26" ht="111" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="49" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="5">
@@ -3063,10 +3053,10 @@
     </row>
     <row r="16" spans="1:26" ht="45">
       <c r="A16" s="1"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="10">
         <v>2</v>
       </c>
@@ -3101,10 +3091,10 @@
     </row>
     <row r="17" spans="1:26" ht="111" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="10">
         <v>3</v>
       </c>
@@ -3139,10 +3129,10 @@
     </row>
     <row r="18" spans="1:26" ht="55.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="10">
         <v>4</v>
       </c>
@@ -3177,10 +3167,10 @@
     </row>
     <row r="19" spans="1:26" ht="105.75" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="10">
         <v>5</v>
       </c>
@@ -3215,10 +3205,10 @@
     </row>
     <row r="20" spans="1:26" ht="45">
       <c r="A20" s="1"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="10">
         <v>6</v>
       </c>
@@ -3319,16 +3309,16 @@
     </row>
     <row r="23" spans="1:26" ht="150">
       <c r="A23" s="1"/>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="49" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="10">
@@ -3365,10 +3355,10 @@
     </row>
     <row r="24" spans="1:26" ht="149.65" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="10">
         <v>2</v>
       </c>
@@ -3403,10 +3393,10 @@
     </row>
     <row r="25" spans="1:26" ht="135.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="10">
         <v>3</v>
       </c>
@@ -3515,10 +3505,10 @@
     </row>
     <row r="28" spans="1:26" ht="45">
       <c r="A28" s="1"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="17">
         <v>2</v>
       </c>
@@ -3553,10 +3543,10 @@
     </row>
     <row r="29" spans="1:26" ht="36" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
       <c r="F29" s="17">
         <v>3</v>
       </c>
@@ -3619,16 +3609,16 @@
     </row>
     <row r="31" spans="1:26" ht="58.15" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="50" t="s">
         <v>56</v>
       </c>
       <c r="F31" s="17">
@@ -3665,10 +3655,10 @@
     </row>
     <row r="32" spans="1:26" ht="57" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="17">
         <v>2</v>
       </c>
@@ -3777,10 +3767,10 @@
     </row>
     <row r="35" spans="1:26" ht="57" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="17">
         <v>2</v>
       </c>
@@ -3815,10 +3805,10 @@
     </row>
     <row r="36" spans="1:26" ht="57" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
       <c r="F36" s="17">
         <v>3</v>
       </c>
@@ -3927,10 +3917,10 @@
     </row>
     <row r="39" spans="1:26" ht="180" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
       <c r="F39" s="17">
         <v>2</v>
       </c>
@@ -3965,7 +3955,7 @@
     </row>
     <row r="40" spans="1:26" ht="189.6" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="39"/>
+      <c r="B40" s="40"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -4029,16 +4019,16 @@
     </row>
     <row r="42" spans="1:26" ht="58.15" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="41" t="s">
         <v>77</v>
       </c>
       <c r="F42" s="17">
@@ -4075,10 +4065,10 @@
     </row>
     <row r="43" spans="1:26" ht="57" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
       <c r="F43" s="17">
         <v>2</v>
       </c>
@@ -4261,10 +4251,10 @@
     </row>
     <row r="48" spans="1:26" ht="57" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
       <c r="F48" s="17">
         <v>2</v>
       </c>
@@ -4299,10 +4289,10 @@
     </row>
     <row r="49" spans="1:26" ht="57" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
       <c r="F49" s="17">
         <v>3</v>
       </c>
@@ -4439,16 +4429,16 @@
     </row>
     <row r="53" spans="1:26" ht="58.15" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="49" t="s">
+      <c r="D53" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="49" t="s">
+      <c r="E53" s="41" t="s">
         <v>94</v>
       </c>
       <c r="F53" s="17">
@@ -4485,10 +4475,10 @@
     </row>
     <row r="54" spans="1:26" ht="58.15" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="17">
         <v>2</v>
       </c>
@@ -4523,10 +4513,10 @@
     </row>
     <row r="55" spans="1:26" ht="58.15" customHeight="1">
       <c r="A55" s="1"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
       <c r="F55" s="17">
         <v>3</v>
       </c>
@@ -4821,10 +4811,10 @@
     </row>
     <row r="63" spans="1:26" ht="53.25" customHeight="1">
       <c r="A63" s="1"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
       <c r="F63" s="17">
         <v>2</v>
       </c>
@@ -5007,10 +4997,10 @@
     </row>
     <row r="68" spans="1:26" ht="50.25" customHeight="1">
       <c r="A68" s="1"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
       <c r="F68" s="17">
         <v>2</v>
       </c>
@@ -5119,10 +5109,10 @@
     </row>
     <row r="71" spans="1:26" ht="34.15" customHeight="1">
       <c r="A71" s="1"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="40"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
       <c r="F71" s="17">
         <v>2</v>
       </c>
@@ -5157,10 +5147,10 @@
     </row>
     <row r="72" spans="1:26" ht="79.5" customHeight="1">
       <c r="A72" s="1"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
       <c r="F72" s="17">
         <v>3</v>
       </c>
@@ -5195,10 +5185,10 @@
     </row>
     <row r="73" spans="1:26" ht="34.15" customHeight="1">
       <c r="A73" s="1"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
       <c r="F73" s="17">
         <v>4</v>
       </c>
@@ -5233,10 +5223,10 @@
     </row>
     <row r="74" spans="1:26" ht="77.25" customHeight="1">
       <c r="A74" s="1"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
       <c r="F74" s="17">
         <v>5</v>
       </c>
@@ -5271,10 +5261,10 @@
     </row>
     <row r="75" spans="1:26" ht="28.9" customHeight="1">
       <c r="A75" s="1"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="40"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
       <c r="F75" s="17">
         <v>6</v>
       </c>
@@ -5309,10 +5299,10 @@
     </row>
     <row r="76" spans="1:26" ht="75.599999999999994" customHeight="1">
       <c r="A76" s="1"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
       <c r="F76" s="17">
         <v>7</v>
       </c>
@@ -5347,10 +5337,10 @@
     </row>
     <row r="77" spans="1:26" ht="29.45" customHeight="1">
       <c r="A77" s="1"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="40"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
       <c r="F77" s="17">
         <v>8</v>
       </c>
@@ -5385,10 +5375,10 @@
     </row>
     <row r="78" spans="1:26" ht="78.75" customHeight="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
       <c r="F78" s="17">
         <v>9</v>
       </c>
@@ -5423,10 +5413,10 @@
     </row>
     <row r="79" spans="1:26" ht="29.45" customHeight="1">
       <c r="A79" s="1"/>
-      <c r="B79" s="40"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="40"/>
-      <c r="E79" s="40"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
       <c r="F79" s="17">
         <v>10</v>
       </c>
@@ -5461,10 +5451,10 @@
     </row>
     <row r="80" spans="1:26" ht="29.45" customHeight="1">
       <c r="A80" s="1"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
+      <c r="D80" s="40"/>
+      <c r="E80" s="40"/>
       <c r="F80" s="17">
         <v>11</v>
       </c>
@@ -5647,10 +5637,10 @@
     </row>
     <row r="85" spans="1:26" ht="45">
       <c r="A85" s="1"/>
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="40"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
       <c r="F85" s="17">
         <v>2</v>
       </c>
@@ -5685,10 +5675,10 @@
     </row>
     <row r="86" spans="1:26" ht="46.9" customHeight="1">
       <c r="A86" s="1"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
       <c r="F86" s="17">
         <v>3</v>
       </c>
@@ -5751,16 +5741,16 @@
     </row>
     <row r="88" spans="1:26" ht="58.15" customHeight="1">
       <c r="A88" s="1"/>
-      <c r="B88" s="45" t="s">
+      <c r="B88" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C88" s="45" t="s">
+      <c r="C88" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="45" t="s">
+      <c r="D88" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="E88" s="45" t="s">
+      <c r="E88" s="50" t="s">
         <v>168</v>
       </c>
       <c r="F88" s="17">
@@ -5797,10 +5787,10 @@
     </row>
     <row r="89" spans="1:26" ht="57" customHeight="1">
       <c r="A89" s="1"/>
-      <c r="B89" s="46"/>
-      <c r="C89" s="46"/>
-      <c r="D89" s="46"/>
-      <c r="E89" s="46"/>
+      <c r="B89" s="51"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="51"/>
+      <c r="E89" s="51"/>
       <c r="F89" s="17">
         <v>2</v>
       </c>
@@ -5909,10 +5899,10 @@
     </row>
     <row r="92" spans="1:26" ht="51" customHeight="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="40"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
       <c r="F92" s="17">
         <v>2</v>
       </c>
@@ -5947,10 +5937,10 @@
     </row>
     <row r="93" spans="1:26" ht="93.6" customHeight="1">
       <c r="A93" s="1"/>
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="40"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
       <c r="F93" s="17">
         <v>3</v>
       </c>
@@ -5985,10 +5975,10 @@
     </row>
     <row r="94" spans="1:26" ht="45" customHeight="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="40"/>
-      <c r="C94" s="40"/>
-      <c r="D94" s="40"/>
-      <c r="E94" s="40"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
       <c r="F94" s="17">
         <v>4</v>
       </c>
@@ -6023,10 +6013,10 @@
     </row>
     <row r="95" spans="1:26" ht="89.45" customHeight="1">
       <c r="A95" s="1"/>
-      <c r="B95" s="40"/>
-      <c r="C95" s="40"/>
-      <c r="D95" s="40"/>
-      <c r="E95" s="40"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
       <c r="F95" s="17">
         <v>5</v>
       </c>
@@ -6061,10 +6051,10 @@
     </row>
     <row r="96" spans="1:26" ht="53.25" customHeight="1">
       <c r="A96" s="1"/>
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="40"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
       <c r="F96" s="17">
         <v>6</v>
       </c>
@@ -6099,10 +6089,10 @@
     </row>
     <row r="97" spans="1:26" ht="39" customHeight="1">
       <c r="A97" s="1"/>
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="40"/>
       <c r="F97" s="17">
         <v>7</v>
       </c>
@@ -6239,16 +6229,16 @@
     </row>
     <row r="101" spans="1:26" ht="123" customHeight="1">
       <c r="A101" s="1"/>
-      <c r="B101" s="41" t="s">
+      <c r="B101" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="C101" s="41" t="s">
+      <c r="C101" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="D101" s="41" t="s">
+      <c r="D101" s="43" t="s">
         <v>248</v>
       </c>
-      <c r="E101" s="41" t="s">
+      <c r="E101" s="43" t="s">
         <v>249</v>
       </c>
       <c r="F101" s="17">
@@ -6285,10 +6275,10 @@
     </row>
     <row r="102" spans="1:26" ht="60">
       <c r="A102" s="1"/>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
+      <c r="B102" s="53"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
       <c r="F102" s="17">
         <v>2</v>
       </c>
@@ -6323,10 +6313,10 @@
     </row>
     <row r="103" spans="1:26" ht="93.6" customHeight="1">
       <c r="A103" s="1"/>
-      <c r="B103" s="47"/>
-      <c r="C103" s="47"/>
-      <c r="D103" s="47"/>
-      <c r="E103" s="47"/>
+      <c r="B103" s="53"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="53"/>
+      <c r="E103" s="53"/>
       <c r="F103" s="17">
         <v>3</v>
       </c>
@@ -6361,10 +6351,10 @@
     </row>
     <row r="104" spans="1:26" ht="60">
       <c r="A104" s="1"/>
-      <c r="B104" s="47"/>
-      <c r="C104" s="47"/>
-      <c r="D104" s="47"/>
-      <c r="E104" s="47"/>
+      <c r="B104" s="53"/>
+      <c r="C104" s="53"/>
+      <c r="D104" s="53"/>
+      <c r="E104" s="53"/>
       <c r="F104" s="17">
         <v>4</v>
       </c>
@@ -6399,10 +6389,10 @@
     </row>
     <row r="105" spans="1:26" ht="75">
       <c r="A105" s="1"/>
-      <c r="B105" s="47"/>
-      <c r="C105" s="47"/>
-      <c r="D105" s="47"/>
-      <c r="E105" s="47"/>
+      <c r="B105" s="53"/>
+      <c r="C105" s="53"/>
+      <c r="D105" s="53"/>
+      <c r="E105" s="53"/>
       <c r="F105" s="17">
         <v>5</v>
       </c>
@@ -6437,10 +6427,10 @@
     </row>
     <row r="106" spans="1:26" ht="60">
       <c r="A106" s="1"/>
-      <c r="B106" s="47"/>
-      <c r="C106" s="47"/>
-      <c r="D106" s="47"/>
-      <c r="E106" s="47"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="53"/>
+      <c r="D106" s="53"/>
+      <c r="E106" s="53"/>
       <c r="F106" s="17">
         <v>6</v>
       </c>
@@ -6475,10 +6465,10 @@
     </row>
     <row r="107" spans="1:26" ht="48.6" customHeight="1">
       <c r="A107" s="1"/>
-      <c r="B107" s="48"/>
-      <c r="C107" s="48"/>
-      <c r="D107" s="48"/>
-      <c r="E107" s="48"/>
+      <c r="B107" s="54"/>
+      <c r="C107" s="54"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="54"/>
       <c r="F107" s="17">
         <v>7</v>
       </c>
@@ -6661,10 +6651,10 @@
     </row>
     <row r="112" spans="1:26" ht="56.25" customHeight="1">
       <c r="A112" s="1"/>
-      <c r="B112" s="40"/>
-      <c r="C112" s="40"/>
-      <c r="D112" s="40"/>
-      <c r="E112" s="40"/>
+      <c r="B112" s="39"/>
+      <c r="C112" s="39"/>
+      <c r="D112" s="39"/>
+      <c r="E112" s="39"/>
       <c r="F112" s="17">
         <v>2</v>
       </c>
@@ -6699,10 +6689,10 @@
     </row>
     <row r="113" spans="1:26" ht="72" customHeight="1">
       <c r="A113" s="1"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="40"/>
+      <c r="D113" s="40"/>
+      <c r="E113" s="40"/>
       <c r="F113" s="17">
         <v>3</v>
       </c>
@@ -6769,7 +6759,7 @@
         <v>185</v>
       </c>
       <c r="C115" s="38" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="D115" s="38" t="s">
         <v>254</v>
@@ -6811,10 +6801,10 @@
     </row>
     <row r="116" spans="1:26" ht="50.25" customHeight="1">
       <c r="A116" s="1"/>
-      <c r="B116" s="40"/>
-      <c r="C116" s="40"/>
-      <c r="D116" s="40"/>
-      <c r="E116" s="40"/>
+      <c r="B116" s="39"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="39"/>
+      <c r="E116" s="39"/>
       <c r="F116" s="17">
         <v>2</v>
       </c>
@@ -6923,10 +6913,10 @@
     </row>
     <row r="119" spans="1:26" ht="46.5" customHeight="1">
       <c r="A119" s="1"/>
-      <c r="B119" s="40"/>
-      <c r="C119" s="40"/>
-      <c r="D119" s="40"/>
-      <c r="E119" s="40"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
       <c r="F119" s="17">
         <v>2</v>
       </c>
@@ -7035,10 +7025,10 @@
     </row>
     <row r="122" spans="1:26" ht="56.25" customHeight="1">
       <c r="A122" s="1"/>
-      <c r="B122" s="40"/>
-      <c r="C122" s="40"/>
-      <c r="D122" s="40"/>
-      <c r="E122" s="40"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
       <c r="F122" s="17">
         <v>2</v>
       </c>
@@ -7073,10 +7063,10 @@
     </row>
     <row r="123" spans="1:26" ht="77.25" customHeight="1">
       <c r="A123" s="1"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="40"/>
+      <c r="E123" s="40"/>
       <c r="F123" s="17">
         <v>3</v>
       </c>
@@ -7185,10 +7175,10 @@
     </row>
     <row r="126" spans="1:26" ht="46.5" customHeight="1">
       <c r="A126" s="1"/>
-      <c r="B126" s="40"/>
-      <c r="C126" s="40"/>
-      <c r="D126" s="40"/>
-      <c r="E126" s="40"/>
+      <c r="B126" s="39"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="39"/>
+      <c r="E126" s="39"/>
       <c r="F126" s="17">
         <v>2</v>
       </c>
@@ -7325,16 +7315,16 @@
     </row>
     <row r="130" spans="1:26" ht="91.5" customHeight="1">
       <c r="A130" s="1"/>
-      <c r="B130" s="41" t="s">
+      <c r="B130" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="C130" s="44" t="s">
+      <c r="C130" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="D130" s="41" t="s">
+      <c r="D130" s="43" t="s">
         <v>272</v>
       </c>
-      <c r="E130" s="41" t="s">
+      <c r="E130" s="43" t="s">
         <v>273</v>
       </c>
       <c r="F130" s="10">
@@ -7371,10 +7361,10 @@
     </row>
     <row r="131" spans="1:26" ht="60.75" customHeight="1">
       <c r="A131" s="1"/>
-      <c r="B131" s="42"/>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="42"/>
+      <c r="B131" s="44"/>
+      <c r="C131" s="44"/>
+      <c r="D131" s="44"/>
+      <c r="E131" s="44"/>
       <c r="F131" s="10">
         <v>2</v>
       </c>
@@ -7595,10 +7585,10 @@
     </row>
     <row r="137" spans="1:26" ht="53.25" customHeight="1">
       <c r="A137" s="1"/>
-      <c r="B137" s="40"/>
-      <c r="C137" s="40"/>
-      <c r="D137" s="40"/>
-      <c r="E137" s="40"/>
+      <c r="B137" s="39"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="39"/>
       <c r="F137" s="17">
         <v>2</v>
       </c>
@@ -7665,7 +7655,7 @@
         <v>289</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>15</v>
+        <v>316</v>
       </c>
       <c r="D139" s="31" t="s">
         <v>286</v>
@@ -7781,10 +7771,10 @@
     </row>
     <row r="142" spans="1:26" ht="56.25" customHeight="1">
       <c r="A142" s="1"/>
-      <c r="B142" s="40"/>
-      <c r="C142" s="40"/>
-      <c r="D142" s="40"/>
-      <c r="E142" s="40"/>
+      <c r="B142" s="39"/>
+      <c r="C142" s="39"/>
+      <c r="D142" s="39"/>
+      <c r="E142" s="39"/>
       <c r="F142" s="17">
         <v>2</v>
       </c>
@@ -7819,10 +7809,10 @@
     </row>
     <row r="143" spans="1:26" ht="96" customHeight="1">
       <c r="A143" s="1"/>
-      <c r="B143" s="39"/>
-      <c r="C143" s="39"/>
-      <c r="D143" s="39"/>
-      <c r="E143" s="39"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="40"/>
+      <c r="D143" s="40"/>
+      <c r="E143" s="40"/>
       <c r="F143" s="17">
         <v>3</v>
       </c>
@@ -7885,16 +7875,16 @@
     </row>
     <row r="145" spans="1:26" ht="111" customHeight="1">
       <c r="A145" s="1"/>
-      <c r="B145" s="41" t="s">
+      <c r="B145" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="44" t="s">
+      <c r="C145" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="D145" s="44" t="s">
+      <c r="D145" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E145" s="41" t="s">
+      <c r="E145" s="43" t="s">
         <v>296</v>
       </c>
       <c r="F145" s="10">
@@ -7931,10 +7921,10 @@
     </row>
     <row r="146" spans="1:26" ht="45">
       <c r="A146" s="1"/>
-      <c r="B146" s="42"/>
-      <c r="C146" s="42"/>
-      <c r="D146" s="42"/>
-      <c r="E146" s="42"/>
+      <c r="B146" s="44"/>
+      <c r="C146" s="44"/>
+      <c r="D146" s="44"/>
+      <c r="E146" s="44"/>
       <c r="F146" s="10">
         <v>2</v>
       </c>
@@ -7969,10 +7959,10 @@
     </row>
     <row r="147" spans="1:26" ht="111" customHeight="1">
       <c r="A147" s="1"/>
-      <c r="B147" s="42"/>
-      <c r="C147" s="42"/>
-      <c r="D147" s="42"/>
-      <c r="E147" s="42"/>
+      <c r="B147" s="44"/>
+      <c r="C147" s="44"/>
+      <c r="D147" s="44"/>
+      <c r="E147" s="44"/>
       <c r="F147" s="10">
         <v>3</v>
       </c>
@@ -8007,10 +7997,10 @@
     </row>
     <row r="148" spans="1:26" ht="55.5" customHeight="1">
       <c r="A148" s="1"/>
-      <c r="B148" s="42"/>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="42"/>
+      <c r="B148" s="44"/>
+      <c r="C148" s="44"/>
+      <c r="D148" s="44"/>
+      <c r="E148" s="44"/>
       <c r="F148" s="10">
         <v>4</v>
       </c>
@@ -8045,10 +8035,10 @@
     </row>
     <row r="149" spans="1:26" ht="105.75" customHeight="1">
       <c r="A149" s="1"/>
-      <c r="B149" s="42"/>
-      <c r="C149" s="42"/>
-      <c r="D149" s="42"/>
-      <c r="E149" s="42"/>
+      <c r="B149" s="44"/>
+      <c r="C149" s="44"/>
+      <c r="D149" s="44"/>
+      <c r="E149" s="44"/>
       <c r="F149" s="10">
         <v>5</v>
       </c>
@@ -8083,10 +8073,10 @@
     </row>
     <row r="150" spans="1:26" ht="45">
       <c r="A150" s="1"/>
-      <c r="B150" s="43"/>
-      <c r="C150" s="43"/>
-      <c r="D150" s="43"/>
-      <c r="E150" s="43"/>
+      <c r="B150" s="45"/>
+      <c r="C150" s="45"/>
+      <c r="D150" s="45"/>
+      <c r="E150" s="45"/>
       <c r="F150" s="10">
         <v>6</v>
       </c>
@@ -8187,16 +8177,16 @@
     </row>
     <row r="153" spans="1:26" ht="135" customHeight="1">
       <c r="A153" s="1"/>
-      <c r="B153" s="41" t="s">
+      <c r="B153" s="43" t="s">
         <v>295</v>
       </c>
       <c r="C153" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="D153" s="44" t="s">
+      <c r="D153" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E153" s="44" t="s">
+      <c r="E153" s="49" t="s">
         <v>35</v>
       </c>
       <c r="F153" s="10">
@@ -8233,10 +8223,10 @@
     </row>
     <row r="154" spans="1:26" ht="149.65" customHeight="1">
       <c r="A154" s="1"/>
-      <c r="B154" s="42"/>
-      <c r="C154" s="40"/>
-      <c r="D154" s="42"/>
-      <c r="E154" s="42"/>
+      <c r="B154" s="44"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="44"/>
+      <c r="E154" s="44"/>
       <c r="F154" s="10">
         <v>2</v>
       </c>
@@ -8271,10 +8261,10 @@
     </row>
     <row r="155" spans="1:26" ht="135.75" customHeight="1">
       <c r="A155" s="1"/>
-      <c r="B155" s="43"/>
-      <c r="C155" s="39"/>
-      <c r="D155" s="43"/>
-      <c r="E155" s="43"/>
+      <c r="B155" s="45"/>
+      <c r="C155" s="40"/>
+      <c r="D155" s="45"/>
+      <c r="E155" s="45"/>
       <c r="F155" s="10">
         <v>3</v>
       </c>
@@ -8383,10 +8373,10 @@
     </row>
     <row r="158" spans="1:26" ht="57" customHeight="1">
       <c r="A158" s="1"/>
-      <c r="B158" s="40"/>
-      <c r="C158" s="40"/>
-      <c r="D158" s="40"/>
-      <c r="E158" s="40"/>
+      <c r="B158" s="39"/>
+      <c r="C158" s="39"/>
+      <c r="D158" s="39"/>
+      <c r="E158" s="39"/>
       <c r="F158" s="17">
         <v>2</v>
       </c>
@@ -8421,10 +8411,10 @@
     </row>
     <row r="159" spans="1:26" ht="57" customHeight="1">
       <c r="A159" s="1"/>
-      <c r="B159" s="39"/>
-      <c r="C159" s="39"/>
-      <c r="D159" s="39"/>
-      <c r="E159" s="39"/>
+      <c r="B159" s="40"/>
+      <c r="C159" s="40"/>
+      <c r="D159" s="40"/>
+      <c r="E159" s="40"/>
       <c r="F159" s="17">
         <v>3</v>
       </c>
@@ -8608,7 +8598,7 @@
     <row r="164" spans="1:26" ht="95.25" customHeight="1">
       <c r="A164" s="1"/>
       <c r="B164" s="30"/>
-      <c r="C164" s="40"/>
+      <c r="C164" s="39"/>
       <c r="D164" s="30"/>
       <c r="E164" s="30"/>
       <c r="F164" s="17">
@@ -8719,10 +8709,10 @@
     </row>
     <row r="167" spans="1:26" ht="44.25" customHeight="1">
       <c r="A167" s="1"/>
-      <c r="B167" s="40"/>
-      <c r="C167" s="40"/>
-      <c r="D167" s="40"/>
-      <c r="E167" s="40"/>
+      <c r="B167" s="39"/>
+      <c r="C167" s="39"/>
+      <c r="D167" s="39"/>
+      <c r="E167" s="39"/>
       <c r="F167" s="17">
         <v>2</v>
       </c>
@@ -8757,10 +8747,10 @@
     </row>
     <row r="168" spans="1:26" ht="79.5" customHeight="1">
       <c r="A168" s="1"/>
-      <c r="B168" s="40"/>
-      <c r="C168" s="40"/>
-      <c r="D168" s="40"/>
-      <c r="E168" s="40"/>
+      <c r="B168" s="39"/>
+      <c r="C168" s="39"/>
+      <c r="D168" s="39"/>
+      <c r="E168" s="39"/>
       <c r="F168" s="17">
         <v>3</v>
       </c>
@@ -8795,10 +8785,10 @@
     </row>
     <row r="169" spans="1:26" ht="46.5" customHeight="1">
       <c r="A169" s="1"/>
-      <c r="B169" s="40"/>
-      <c r="C169" s="40"/>
-      <c r="D169" s="40"/>
-      <c r="E169" s="40"/>
+      <c r="B169" s="39"/>
+      <c r="C169" s="39"/>
+      <c r="D169" s="39"/>
+      <c r="E169" s="39"/>
       <c r="F169" s="17">
         <v>4</v>
       </c>
@@ -8833,10 +8823,10 @@
     </row>
     <row r="170" spans="1:26" ht="75" customHeight="1">
       <c r="A170" s="1"/>
-      <c r="B170" s="40"/>
-      <c r="C170" s="40"/>
-      <c r="D170" s="40"/>
-      <c r="E170" s="40"/>
+      <c r="B170" s="39"/>
+      <c r="C170" s="39"/>
+      <c r="D170" s="39"/>
+      <c r="E170" s="39"/>
       <c r="F170" s="17">
         <v>5</v>
       </c>
@@ -8871,10 +8861,10 @@
     </row>
     <row r="171" spans="1:26" ht="51.75" customHeight="1">
       <c r="A171" s="1"/>
-      <c r="B171" s="40"/>
-      <c r="C171" s="40"/>
-      <c r="D171" s="40"/>
-      <c r="E171" s="40"/>
+      <c r="B171" s="39"/>
+      <c r="C171" s="39"/>
+      <c r="D171" s="39"/>
+      <c r="E171" s="39"/>
       <c r="F171" s="17">
         <v>6</v>
       </c>
@@ -8909,10 +8899,10 @@
     </row>
     <row r="172" spans="1:26" ht="45.75" customHeight="1">
       <c r="A172" s="1"/>
-      <c r="B172" s="39"/>
-      <c r="C172" s="39"/>
-      <c r="D172" s="39"/>
-      <c r="E172" s="39"/>
+      <c r="B172" s="40"/>
+      <c r="C172" s="40"/>
+      <c r="D172" s="40"/>
+      <c r="E172" s="40"/>
       <c r="F172" s="17">
         <v>7</v>
       </c>
@@ -9095,10 +9085,10 @@
     </row>
     <row r="177" spans="1:26" ht="66" customHeight="1">
       <c r="A177" s="1"/>
-      <c r="B177" s="39"/>
-      <c r="C177" s="39"/>
-      <c r="D177" s="39"/>
-      <c r="E177" s="39"/>
+      <c r="B177" s="40"/>
+      <c r="C177" s="40"/>
+      <c r="D177" s="40"/>
+      <c r="E177" s="40"/>
       <c r="F177" s="17">
         <v>2</v>
       </c>
@@ -9133,84 +9123,31 @@
     </row>
   </sheetData>
   <mergeCells count="127">
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="E91:E97"/>
-    <mergeCell ref="D91:D97"/>
-    <mergeCell ref="C91:C97"/>
-    <mergeCell ref="B91:B97"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="E70:E80"/>
-    <mergeCell ref="D70:D80"/>
-    <mergeCell ref="C70:C80"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="E84:E86"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B101:B107"/>
-    <mergeCell ref="C101:C107"/>
-    <mergeCell ref="D101:D107"/>
-    <mergeCell ref="E101:E107"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="D176:D177"/>
+    <mergeCell ref="E176:E177"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="D157:D159"/>
+    <mergeCell ref="E157:E159"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B166:B172"/>
+    <mergeCell ref="C166:C172"/>
+    <mergeCell ref="D166:D172"/>
+    <mergeCell ref="E166:E172"/>
+    <mergeCell ref="B141:B143"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="D141:D143"/>
+    <mergeCell ref="E141:E143"/>
+    <mergeCell ref="B145:B150"/>
+    <mergeCell ref="C145:C150"/>
+    <mergeCell ref="D145:D150"/>
+    <mergeCell ref="E145:E150"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="D153:D155"/>
+    <mergeCell ref="E153:E155"/>
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="C121:C123"/>
     <mergeCell ref="D121:D123"/>
@@ -9235,31 +9172,84 @@
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="C125:C126"/>
     <mergeCell ref="D125:D126"/>
-    <mergeCell ref="B141:B143"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="D141:D143"/>
-    <mergeCell ref="E141:E143"/>
-    <mergeCell ref="B145:B150"/>
-    <mergeCell ref="C145:C150"/>
-    <mergeCell ref="D145:D150"/>
-    <mergeCell ref="E145:E150"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="D153:D155"/>
-    <mergeCell ref="E153:E155"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="D176:D177"/>
-    <mergeCell ref="E176:E177"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="D157:D159"/>
-    <mergeCell ref="E157:E159"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B166:B172"/>
-    <mergeCell ref="C166:C172"/>
-    <mergeCell ref="D166:D172"/>
-    <mergeCell ref="E166:E172"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="E70:E80"/>
+    <mergeCell ref="D70:D80"/>
+    <mergeCell ref="C70:C80"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E91:E97"/>
+    <mergeCell ref="D91:D97"/>
+    <mergeCell ref="C91:C97"/>
+    <mergeCell ref="B91:B97"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="E84:E86"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B101:B107"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="D101:D107"/>
+    <mergeCell ref="E101:E107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Terminados Casos de uso
</commit_message>
<xml_diff>
--- a/Documentacion/Plantilla Historias Usuario - Oficina de Proyectos de Informatica.xlsx
+++ b/Documentacion/Plantilla Historias Usuario - Oficina de Proyectos de Informatica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\E-vote\E-vote-Backend\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACAA4A5-4664-47C4-B562-1F40CDDC15F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D411CC5-55BE-4B5B-8B1C-7587B30B4E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -2088,17 +2088,11 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2109,21 +2103,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2474,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J119" sqref="J119"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J131" sqref="J131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2592,18 +2592,18 @@
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="46" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2715,10 +2715,10 @@
     </row>
     <row r="7" spans="1:26" ht="57" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="17">
         <v>2</v>
       </c>
@@ -2753,10 +2753,10 @@
     </row>
     <row r="8" spans="1:26" ht="131.25" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="17">
         <v>3</v>
       </c>
@@ -2819,16 +2819,16 @@
     </row>
     <row r="10" spans="1:26" ht="45">
       <c r="A10" s="1"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="5">
@@ -2865,10 +2865,10 @@
     </row>
     <row r="11" spans="1:26" ht="52.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="5">
         <v>2</v>
       </c>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="10">
         <v>3</v>
       </c>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="13" spans="1:26" ht="49.9" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="10">
         <v>4</v>
       </c>
@@ -3007,16 +3007,16 @@
     </row>
     <row r="15" spans="1:26" ht="111" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="44" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="5">
@@ -3053,10 +3053,10 @@
     </row>
     <row r="16" spans="1:26" ht="45">
       <c r="A16" s="1"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="10">
         <v>2</v>
       </c>
@@ -3091,10 +3091,10 @@
     </row>
     <row r="17" spans="1:26" ht="111" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="10">
         <v>3</v>
       </c>
@@ -3129,10 +3129,10 @@
     </row>
     <row r="18" spans="1:26" ht="55.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="10">
         <v>4</v>
       </c>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="19" spans="1:26" ht="105.75" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="10">
         <v>5</v>
       </c>
@@ -3205,10 +3205,10 @@
     </row>
     <row r="20" spans="1:26" ht="45">
       <c r="A20" s="1"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="10">
         <v>6</v>
       </c>
@@ -3309,16 +3309,16 @@
     </row>
     <row r="23" spans="1:26" ht="150">
       <c r="A23" s="1"/>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="49" t="s">
+      <c r="E23" s="44" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="10">
@@ -3355,10 +3355,10 @@
     </row>
     <row r="24" spans="1:26" ht="149.65" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="10">
         <v>2</v>
       </c>
@@ -3393,10 +3393,10 @@
     </row>
     <row r="25" spans="1:26" ht="135.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="10">
         <v>3</v>
       </c>
@@ -3505,10 +3505,10 @@
     </row>
     <row r="28" spans="1:26" ht="45">
       <c r="A28" s="1"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="17">
         <v>2</v>
       </c>
@@ -3543,10 +3543,10 @@
     </row>
     <row r="29" spans="1:26" ht="36" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="17">
         <v>3</v>
       </c>
@@ -3609,16 +3609,16 @@
     </row>
     <row r="31" spans="1:26" ht="58.15" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="51" t="s">
         <v>56</v>
       </c>
       <c r="F31" s="17">
@@ -3655,10 +3655,10 @@
     </row>
     <row r="32" spans="1:26" ht="57" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
       <c r="F32" s="17">
         <v>2</v>
       </c>
@@ -3767,10 +3767,10 @@
     </row>
     <row r="35" spans="1:26" ht="57" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="17">
         <v>2</v>
       </c>
@@ -3805,10 +3805,10 @@
     </row>
     <row r="36" spans="1:26" ht="57" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="17">
         <v>3</v>
       </c>
@@ -3917,10 +3917,10 @@
     </row>
     <row r="39" spans="1:26" ht="180" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="17">
         <v>2</v>
       </c>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="40" spans="1:26" ht="189.6" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="40"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -4019,16 +4019,16 @@
     </row>
     <row r="42" spans="1:26" ht="58.15" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="41" t="s">
+      <c r="D42" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="45" t="s">
         <v>77</v>
       </c>
       <c r="F42" s="17">
@@ -4065,10 +4065,10 @@
     </row>
     <row r="43" spans="1:26" ht="57" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="17">
         <v>2</v>
       </c>
@@ -4251,10 +4251,10 @@
     </row>
     <row r="48" spans="1:26" ht="57" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
       <c r="F48" s="17">
         <v>2</v>
       </c>
@@ -4289,10 +4289,10 @@
     </row>
     <row r="49" spans="1:26" ht="57" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
       <c r="F49" s="17">
         <v>3</v>
       </c>
@@ -4429,16 +4429,16 @@
     </row>
     <row r="53" spans="1:26" ht="58.15" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="41" t="s">
+      <c r="D53" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="45" t="s">
         <v>94</v>
       </c>
       <c r="F53" s="17">
@@ -4475,10 +4475,10 @@
     </row>
     <row r="54" spans="1:26" ht="58.15" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
       <c r="F54" s="17">
         <v>2</v>
       </c>
@@ -4513,10 +4513,10 @@
     </row>
     <row r="55" spans="1:26" ht="58.15" customHeight="1">
       <c r="A55" s="1"/>
-      <c r="B55" s="42"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
       <c r="F55" s="17">
         <v>3</v>
       </c>
@@ -4811,10 +4811,10 @@
     </row>
     <row r="63" spans="1:26" ht="53.25" customHeight="1">
       <c r="A63" s="1"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
       <c r="F63" s="17">
         <v>2</v>
       </c>
@@ -4997,10 +4997,10 @@
     </row>
     <row r="68" spans="1:26" ht="50.25" customHeight="1">
       <c r="A68" s="1"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="40"/>
       <c r="F68" s="17">
         <v>2</v>
       </c>
@@ -5109,10 +5109,10 @@
     </row>
     <row r="71" spans="1:26" ht="34.15" customHeight="1">
       <c r="A71" s="1"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
       <c r="F71" s="17">
         <v>2</v>
       </c>
@@ -5147,10 +5147,10 @@
     </row>
     <row r="72" spans="1:26" ht="79.5" customHeight="1">
       <c r="A72" s="1"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
       <c r="F72" s="17">
         <v>3</v>
       </c>
@@ -5185,10 +5185,10 @@
     </row>
     <row r="73" spans="1:26" ht="34.15" customHeight="1">
       <c r="A73" s="1"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="40"/>
       <c r="F73" s="17">
         <v>4</v>
       </c>
@@ -5223,10 +5223,10 @@
     </row>
     <row r="74" spans="1:26" ht="77.25" customHeight="1">
       <c r="A74" s="1"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="40"/>
       <c r="F74" s="17">
         <v>5</v>
       </c>
@@ -5261,10 +5261,10 @@
     </row>
     <row r="75" spans="1:26" ht="28.9" customHeight="1">
       <c r="A75" s="1"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
       <c r="F75" s="17">
         <v>6</v>
       </c>
@@ -5299,10 +5299,10 @@
     </row>
     <row r="76" spans="1:26" ht="75.599999999999994" customHeight="1">
       <c r="A76" s="1"/>
-      <c r="B76" s="39"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="40"/>
       <c r="F76" s="17">
         <v>7</v>
       </c>
@@ -5337,10 +5337,10 @@
     </row>
     <row r="77" spans="1:26" ht="29.45" customHeight="1">
       <c r="A77" s="1"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="40"/>
       <c r="F77" s="17">
         <v>8</v>
       </c>
@@ -5375,10 +5375,10 @@
     </row>
     <row r="78" spans="1:26" ht="78.75" customHeight="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
       <c r="F78" s="17">
         <v>9</v>
       </c>
@@ -5413,10 +5413,10 @@
     </row>
     <row r="79" spans="1:26" ht="29.45" customHeight="1">
       <c r="A79" s="1"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="40"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
       <c r="F79" s="17">
         <v>10</v>
       </c>
@@ -5451,10 +5451,10 @@
     </row>
     <row r="80" spans="1:26" ht="29.45" customHeight="1">
       <c r="A80" s="1"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="40"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
       <c r="F80" s="17">
         <v>11</v>
       </c>
@@ -5637,10 +5637,10 @@
     </row>
     <row r="85" spans="1:26" ht="45">
       <c r="A85" s="1"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="40"/>
       <c r="F85" s="17">
         <v>2</v>
       </c>
@@ -5675,10 +5675,10 @@
     </row>
     <row r="86" spans="1:26" ht="46.9" customHeight="1">
       <c r="A86" s="1"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="40"/>
       <c r="F86" s="17">
         <v>3</v>
       </c>
@@ -5741,16 +5741,16 @@
     </row>
     <row r="88" spans="1:26" ht="58.15" customHeight="1">
       <c r="A88" s="1"/>
-      <c r="B88" s="50" t="s">
+      <c r="B88" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="C88" s="50" t="s">
+      <c r="C88" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="50" t="s">
+      <c r="D88" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="E88" s="50" t="s">
+      <c r="E88" s="51" t="s">
         <v>168</v>
       </c>
       <c r="F88" s="17">
@@ -5787,10 +5787,10 @@
     </row>
     <row r="89" spans="1:26" ht="57" customHeight="1">
       <c r="A89" s="1"/>
-      <c r="B89" s="51"/>
-      <c r="C89" s="51"/>
-      <c r="D89" s="51"/>
-      <c r="E89" s="51"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="52"/>
+      <c r="D89" s="52"/>
+      <c r="E89" s="52"/>
       <c r="F89" s="17">
         <v>2</v>
       </c>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="92" spans="1:26" ht="51" customHeight="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="39"/>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="40"/>
       <c r="F92" s="17">
         <v>2</v>
       </c>
@@ -5937,10 +5937,10 @@
     </row>
     <row r="93" spans="1:26" ht="93.6" customHeight="1">
       <c r="A93" s="1"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="40"/>
       <c r="F93" s="17">
         <v>3</v>
       </c>
@@ -5975,10 +5975,10 @@
     </row>
     <row r="94" spans="1:26" ht="45" customHeight="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
+      <c r="E94" s="40"/>
       <c r="F94" s="17">
         <v>4</v>
       </c>
@@ -6013,10 +6013,10 @@
     </row>
     <row r="95" spans="1:26" ht="89.45" customHeight="1">
       <c r="A95" s="1"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="40"/>
       <c r="F95" s="17">
         <v>5</v>
       </c>
@@ -6051,10 +6051,10 @@
     </row>
     <row r="96" spans="1:26" ht="53.25" customHeight="1">
       <c r="A96" s="1"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="40"/>
       <c r="F96" s="17">
         <v>6</v>
       </c>
@@ -6089,10 +6089,10 @@
     </row>
     <row r="97" spans="1:26" ht="39" customHeight="1">
       <c r="A97" s="1"/>
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="40"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
+      <c r="E97" s="39"/>
       <c r="F97" s="17">
         <v>7</v>
       </c>
@@ -6229,16 +6229,16 @@
     </row>
     <row r="101" spans="1:26" ht="123" customHeight="1">
       <c r="A101" s="1"/>
-      <c r="B101" s="43" t="s">
+      <c r="B101" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="C101" s="43" t="s">
+      <c r="C101" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="D101" s="43" t="s">
+      <c r="D101" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="E101" s="43" t="s">
+      <c r="E101" s="41" t="s">
         <v>249</v>
       </c>
       <c r="F101" s="17">
@@ -6651,10 +6651,10 @@
     </row>
     <row r="112" spans="1:26" ht="56.25" customHeight="1">
       <c r="A112" s="1"/>
-      <c r="B112" s="39"/>
-      <c r="C112" s="39"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="40"/>
+      <c r="D112" s="40"/>
+      <c r="E112" s="40"/>
       <c r="F112" s="17">
         <v>2</v>
       </c>
@@ -6689,10 +6689,10 @@
     </row>
     <row r="113" spans="1:26" ht="72" customHeight="1">
       <c r="A113" s="1"/>
-      <c r="B113" s="40"/>
-      <c r="C113" s="40"/>
-      <c r="D113" s="40"/>
-      <c r="E113" s="40"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
+      <c r="E113" s="39"/>
       <c r="F113" s="17">
         <v>3</v>
       </c>
@@ -6801,10 +6801,10 @@
     </row>
     <row r="116" spans="1:26" ht="50.25" customHeight="1">
       <c r="A116" s="1"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
+      <c r="E116" s="40"/>
       <c r="F116" s="17">
         <v>2</v>
       </c>
@@ -6913,10 +6913,10 @@
     </row>
     <row r="119" spans="1:26" ht="46.5" customHeight="1">
       <c r="A119" s="1"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
+      <c r="E119" s="40"/>
       <c r="F119" s="17">
         <v>2</v>
       </c>
@@ -7025,10 +7025,10 @@
     </row>
     <row r="122" spans="1:26" ht="56.25" customHeight="1">
       <c r="A122" s="1"/>
-      <c r="B122" s="39"/>
-      <c r="C122" s="39"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="39"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
+      <c r="E122" s="40"/>
       <c r="F122" s="17">
         <v>2</v>
       </c>
@@ -7063,10 +7063,10 @@
     </row>
     <row r="123" spans="1:26" ht="77.25" customHeight="1">
       <c r="A123" s="1"/>
-      <c r="B123" s="40"/>
-      <c r="C123" s="40"/>
-      <c r="D123" s="40"/>
-      <c r="E123" s="40"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="39"/>
+      <c r="E123" s="39"/>
       <c r="F123" s="17">
         <v>3</v>
       </c>
@@ -7175,10 +7175,10 @@
     </row>
     <row r="126" spans="1:26" ht="46.5" customHeight="1">
       <c r="A126" s="1"/>
-      <c r="B126" s="39"/>
-      <c r="C126" s="39"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="39"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
+      <c r="D126" s="40"/>
+      <c r="E126" s="40"/>
       <c r="F126" s="17">
         <v>2</v>
       </c>
@@ -7315,16 +7315,16 @@
     </row>
     <row r="130" spans="1:26" ht="91.5" customHeight="1">
       <c r="A130" s="1"/>
-      <c r="B130" s="43" t="s">
+      <c r="B130" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="C130" s="49" t="s">
+      <c r="C130" s="44" t="s">
         <v>263</v>
       </c>
-      <c r="D130" s="43" t="s">
+      <c r="D130" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="E130" s="43" t="s">
+      <c r="E130" s="41" t="s">
         <v>273</v>
       </c>
       <c r="F130" s="10">
@@ -7361,10 +7361,10 @@
     </row>
     <row r="131" spans="1:26" ht="60.75" customHeight="1">
       <c r="A131" s="1"/>
-      <c r="B131" s="44"/>
-      <c r="C131" s="44"/>
-      <c r="D131" s="44"/>
-      <c r="E131" s="44"/>
+      <c r="B131" s="42"/>
+      <c r="C131" s="42"/>
+      <c r="D131" s="42"/>
+      <c r="E131" s="42"/>
       <c r="F131" s="10">
         <v>2</v>
       </c>
@@ -7585,10 +7585,10 @@
     </row>
     <row r="137" spans="1:26" ht="53.25" customHeight="1">
       <c r="A137" s="1"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="39"/>
-      <c r="D137" s="39"/>
-      <c r="E137" s="39"/>
+      <c r="B137" s="40"/>
+      <c r="C137" s="40"/>
+      <c r="D137" s="40"/>
+      <c r="E137" s="40"/>
       <c r="F137" s="17">
         <v>2</v>
       </c>
@@ -7771,10 +7771,10 @@
     </row>
     <row r="142" spans="1:26" ht="56.25" customHeight="1">
       <c r="A142" s="1"/>
-      <c r="B142" s="39"/>
-      <c r="C142" s="39"/>
-      <c r="D142" s="39"/>
-      <c r="E142" s="39"/>
+      <c r="B142" s="40"/>
+      <c r="C142" s="40"/>
+      <c r="D142" s="40"/>
+      <c r="E142" s="40"/>
       <c r="F142" s="17">
         <v>2</v>
       </c>
@@ -7809,10 +7809,10 @@
     </row>
     <row r="143" spans="1:26" ht="96" customHeight="1">
       <c r="A143" s="1"/>
-      <c r="B143" s="40"/>
-      <c r="C143" s="40"/>
-      <c r="D143" s="40"/>
-      <c r="E143" s="40"/>
+      <c r="B143" s="39"/>
+      <c r="C143" s="39"/>
+      <c r="D143" s="39"/>
+      <c r="E143" s="39"/>
       <c r="F143" s="17">
         <v>3</v>
       </c>
@@ -7875,16 +7875,16 @@
     </row>
     <row r="145" spans="1:26" ht="111" customHeight="1">
       <c r="A145" s="1"/>
-      <c r="B145" s="43" t="s">
+      <c r="B145" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="49" t="s">
+      <c r="C145" s="44" t="s">
         <v>290</v>
       </c>
-      <c r="D145" s="49" t="s">
+      <c r="D145" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E145" s="43" t="s">
+      <c r="E145" s="41" t="s">
         <v>296</v>
       </c>
       <c r="F145" s="10">
@@ -7921,10 +7921,10 @@
     </row>
     <row r="146" spans="1:26" ht="45">
       <c r="A146" s="1"/>
-      <c r="B146" s="44"/>
-      <c r="C146" s="44"/>
-      <c r="D146" s="44"/>
-      <c r="E146" s="44"/>
+      <c r="B146" s="42"/>
+      <c r="C146" s="42"/>
+      <c r="D146" s="42"/>
+      <c r="E146" s="42"/>
       <c r="F146" s="10">
         <v>2</v>
       </c>
@@ -7959,10 +7959,10 @@
     </row>
     <row r="147" spans="1:26" ht="111" customHeight="1">
       <c r="A147" s="1"/>
-      <c r="B147" s="44"/>
-      <c r="C147" s="44"/>
-      <c r="D147" s="44"/>
-      <c r="E147" s="44"/>
+      <c r="B147" s="42"/>
+      <c r="C147" s="42"/>
+      <c r="D147" s="42"/>
+      <c r="E147" s="42"/>
       <c r="F147" s="10">
         <v>3</v>
       </c>
@@ -7997,10 +7997,10 @@
     </row>
     <row r="148" spans="1:26" ht="55.5" customHeight="1">
       <c r="A148" s="1"/>
-      <c r="B148" s="44"/>
-      <c r="C148" s="44"/>
-      <c r="D148" s="44"/>
-      <c r="E148" s="44"/>
+      <c r="B148" s="42"/>
+      <c r="C148" s="42"/>
+      <c r="D148" s="42"/>
+      <c r="E148" s="42"/>
       <c r="F148" s="10">
         <v>4</v>
       </c>
@@ -8035,10 +8035,10 @@
     </row>
     <row r="149" spans="1:26" ht="105.75" customHeight="1">
       <c r="A149" s="1"/>
-      <c r="B149" s="44"/>
-      <c r="C149" s="44"/>
-      <c r="D149" s="44"/>
-      <c r="E149" s="44"/>
+      <c r="B149" s="42"/>
+      <c r="C149" s="42"/>
+      <c r="D149" s="42"/>
+      <c r="E149" s="42"/>
       <c r="F149" s="10">
         <v>5</v>
       </c>
@@ -8073,10 +8073,10 @@
     </row>
     <row r="150" spans="1:26" ht="45">
       <c r="A150" s="1"/>
-      <c r="B150" s="45"/>
-      <c r="C150" s="45"/>
-      <c r="D150" s="45"/>
-      <c r="E150" s="45"/>
+      <c r="B150" s="43"/>
+      <c r="C150" s="43"/>
+      <c r="D150" s="43"/>
+      <c r="E150" s="43"/>
       <c r="F150" s="10">
         <v>6</v>
       </c>
@@ -8177,16 +8177,16 @@
     </row>
     <row r="153" spans="1:26" ht="135" customHeight="1">
       <c r="A153" s="1"/>
-      <c r="B153" s="43" t="s">
+      <c r="B153" s="41" t="s">
         <v>295</v>
       </c>
       <c r="C153" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="D153" s="49" t="s">
+      <c r="D153" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E153" s="49" t="s">
+      <c r="E153" s="44" t="s">
         <v>35</v>
       </c>
       <c r="F153" s="10">
@@ -8223,10 +8223,10 @@
     </row>
     <row r="154" spans="1:26" ht="149.65" customHeight="1">
       <c r="A154" s="1"/>
-      <c r="B154" s="44"/>
-      <c r="C154" s="39"/>
-      <c r="D154" s="44"/>
-      <c r="E154" s="44"/>
+      <c r="B154" s="42"/>
+      <c r="C154" s="40"/>
+      <c r="D154" s="42"/>
+      <c r="E154" s="42"/>
       <c r="F154" s="10">
         <v>2</v>
       </c>
@@ -8261,10 +8261,10 @@
     </row>
     <row r="155" spans="1:26" ht="135.75" customHeight="1">
       <c r="A155" s="1"/>
-      <c r="B155" s="45"/>
-      <c r="C155" s="40"/>
-      <c r="D155" s="45"/>
-      <c r="E155" s="45"/>
+      <c r="B155" s="43"/>
+      <c r="C155" s="39"/>
+      <c r="D155" s="43"/>
+      <c r="E155" s="43"/>
       <c r="F155" s="10">
         <v>3</v>
       </c>
@@ -8373,10 +8373,10 @@
     </row>
     <row r="158" spans="1:26" ht="57" customHeight="1">
       <c r="A158" s="1"/>
-      <c r="B158" s="39"/>
-      <c r="C158" s="39"/>
-      <c r="D158" s="39"/>
-      <c r="E158" s="39"/>
+      <c r="B158" s="40"/>
+      <c r="C158" s="40"/>
+      <c r="D158" s="40"/>
+      <c r="E158" s="40"/>
       <c r="F158" s="17">
         <v>2</v>
       </c>
@@ -8411,10 +8411,10 @@
     </row>
     <row r="159" spans="1:26" ht="57" customHeight="1">
       <c r="A159" s="1"/>
-      <c r="B159" s="40"/>
-      <c r="C159" s="40"/>
-      <c r="D159" s="40"/>
-      <c r="E159" s="40"/>
+      <c r="B159" s="39"/>
+      <c r="C159" s="39"/>
+      <c r="D159" s="39"/>
+      <c r="E159" s="39"/>
       <c r="F159" s="17">
         <v>3</v>
       </c>
@@ -8598,7 +8598,7 @@
     <row r="164" spans="1:26" ht="95.25" customHeight="1">
       <c r="A164" s="1"/>
       <c r="B164" s="30"/>
-      <c r="C164" s="39"/>
+      <c r="C164" s="40"/>
       <c r="D164" s="30"/>
       <c r="E164" s="30"/>
       <c r="F164" s="17">
@@ -8709,10 +8709,10 @@
     </row>
     <row r="167" spans="1:26" ht="44.25" customHeight="1">
       <c r="A167" s="1"/>
-      <c r="B167" s="39"/>
-      <c r="C167" s="39"/>
-      <c r="D167" s="39"/>
-      <c r="E167" s="39"/>
+      <c r="B167" s="40"/>
+      <c r="C167" s="40"/>
+      <c r="D167" s="40"/>
+      <c r="E167" s="40"/>
       <c r="F167" s="17">
         <v>2</v>
       </c>
@@ -8747,10 +8747,10 @@
     </row>
     <row r="168" spans="1:26" ht="79.5" customHeight="1">
       <c r="A168" s="1"/>
-      <c r="B168" s="39"/>
-      <c r="C168" s="39"/>
-      <c r="D168" s="39"/>
-      <c r="E168" s="39"/>
+      <c r="B168" s="40"/>
+      <c r="C168" s="40"/>
+      <c r="D168" s="40"/>
+      <c r="E168" s="40"/>
       <c r="F168" s="17">
         <v>3</v>
       </c>
@@ -8785,10 +8785,10 @@
     </row>
     <row r="169" spans="1:26" ht="46.5" customHeight="1">
       <c r="A169" s="1"/>
-      <c r="B169" s="39"/>
-      <c r="C169" s="39"/>
-      <c r="D169" s="39"/>
-      <c r="E169" s="39"/>
+      <c r="B169" s="40"/>
+      <c r="C169" s="40"/>
+      <c r="D169" s="40"/>
+      <c r="E169" s="40"/>
       <c r="F169" s="17">
         <v>4</v>
       </c>
@@ -8823,10 +8823,10 @@
     </row>
     <row r="170" spans="1:26" ht="75" customHeight="1">
       <c r="A170" s="1"/>
-      <c r="B170" s="39"/>
-      <c r="C170" s="39"/>
-      <c r="D170" s="39"/>
-      <c r="E170" s="39"/>
+      <c r="B170" s="40"/>
+      <c r="C170" s="40"/>
+      <c r="D170" s="40"/>
+      <c r="E170" s="40"/>
       <c r="F170" s="17">
         <v>5</v>
       </c>
@@ -8861,10 +8861,10 @@
     </row>
     <row r="171" spans="1:26" ht="51.75" customHeight="1">
       <c r="A171" s="1"/>
-      <c r="B171" s="39"/>
-      <c r="C171" s="39"/>
-      <c r="D171" s="39"/>
-      <c r="E171" s="39"/>
+      <c r="B171" s="40"/>
+      <c r="C171" s="40"/>
+      <c r="D171" s="40"/>
+      <c r="E171" s="40"/>
       <c r="F171" s="17">
         <v>6</v>
       </c>
@@ -8899,10 +8899,10 @@
     </row>
     <row r="172" spans="1:26" ht="45.75" customHeight="1">
       <c r="A172" s="1"/>
-      <c r="B172" s="40"/>
-      <c r="C172" s="40"/>
-      <c r="D172" s="40"/>
-      <c r="E172" s="40"/>
+      <c r="B172" s="39"/>
+      <c r="C172" s="39"/>
+      <c r="D172" s="39"/>
+      <c r="E172" s="39"/>
       <c r="F172" s="17">
         <v>7</v>
       </c>
@@ -9085,10 +9085,10 @@
     </row>
     <row r="177" spans="1:26" ht="66" customHeight="1">
       <c r="A177" s="1"/>
-      <c r="B177" s="40"/>
-      <c r="C177" s="40"/>
-      <c r="D177" s="40"/>
-      <c r="E177" s="40"/>
+      <c r="B177" s="39"/>
+      <c r="C177" s="39"/>
+      <c r="D177" s="39"/>
+      <c r="E177" s="39"/>
       <c r="F177" s="17">
         <v>2</v>
       </c>
@@ -9123,31 +9123,84 @@
     </row>
   </sheetData>
   <mergeCells count="127">
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="D176:D177"/>
-    <mergeCell ref="E176:E177"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="D157:D159"/>
-    <mergeCell ref="E157:E159"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B166:B172"/>
-    <mergeCell ref="C166:C172"/>
-    <mergeCell ref="D166:D172"/>
-    <mergeCell ref="E166:E172"/>
-    <mergeCell ref="B141:B143"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="D141:D143"/>
-    <mergeCell ref="E141:E143"/>
-    <mergeCell ref="B145:B150"/>
-    <mergeCell ref="C145:C150"/>
-    <mergeCell ref="D145:D150"/>
-    <mergeCell ref="E145:E150"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="D153:D155"/>
-    <mergeCell ref="E153:E155"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E91:E97"/>
+    <mergeCell ref="D91:D97"/>
+    <mergeCell ref="C91:C97"/>
+    <mergeCell ref="B91:B97"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="E84:E86"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B101:B107"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="D101:D107"/>
+    <mergeCell ref="E101:E107"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="B70:B80"/>
+    <mergeCell ref="E70:E80"/>
+    <mergeCell ref="D70:D80"/>
+    <mergeCell ref="C70:C80"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="C121:C123"/>
     <mergeCell ref="D121:D123"/>
@@ -9172,84 +9225,31 @@
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="C125:C126"/>
     <mergeCell ref="D125:D126"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="B70:B80"/>
-    <mergeCell ref="E70:E80"/>
-    <mergeCell ref="D70:D80"/>
-    <mergeCell ref="C70:C80"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="E91:E97"/>
-    <mergeCell ref="D91:D97"/>
-    <mergeCell ref="C91:C97"/>
-    <mergeCell ref="B91:B97"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="E84:E86"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B101:B107"/>
-    <mergeCell ref="C101:C107"/>
-    <mergeCell ref="D101:D107"/>
-    <mergeCell ref="E101:E107"/>
+    <mergeCell ref="B141:B143"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="D141:D143"/>
+    <mergeCell ref="E141:E143"/>
+    <mergeCell ref="B145:B150"/>
+    <mergeCell ref="C145:C150"/>
+    <mergeCell ref="D145:D150"/>
+    <mergeCell ref="E145:E150"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="D153:D155"/>
+    <mergeCell ref="E153:E155"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="D176:D177"/>
+    <mergeCell ref="E176:E177"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="D157:D159"/>
+    <mergeCell ref="E157:E159"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B166:B172"/>
+    <mergeCell ref="C166:C172"/>
+    <mergeCell ref="D166:D172"/>
+    <mergeCell ref="E166:E172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>